<commit_message>
Correção dos incadores de prazos e ciclos
</commit_message>
<xml_diff>
--- a/planilhas/Indicadores_Financeiros_Embraer.xlsx
+++ b/planilhas/Indicadores_Financeiros_Embraer.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,19 +458,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.61068036787363</v>
+        <v>3.61068036787363</v>
       </c>
       <c r="C2" t="n">
-        <v>2.65978964066897</v>
+        <v>3.65978964066897</v>
       </c>
       <c r="D2" t="n">
-        <v>2.590901228701166</v>
+        <v>3.590901228701167</v>
       </c>
       <c r="E2" t="n">
-        <v>2.547669704768785</v>
+        <v>3.547669704768785</v>
       </c>
       <c r="F2" t="n">
-        <v>2.535321483732147</v>
+        <v>3.535321483732147</v>
       </c>
     </row>
     <row r="3">
@@ -480,19 +480,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72.30438869921596</v>
+        <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>72.67602517675823</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>72.15183776130478</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
-        <v>71.81248303200837</v>
+        <v>100</v>
       </c>
       <c r="F3" t="n">
-        <v>71.71402927282512</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -524,19 +524,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.777338748265412</v>
+        <v>2.61068036787363</v>
       </c>
       <c r="C5" t="n">
-        <v>1.640271672050957</v>
+        <v>2.65978964066897</v>
       </c>
       <c r="D5" t="n">
-        <v>1.451796019768496</v>
+        <v>2.590901228701166</v>
       </c>
       <c r="E5" t="n">
-        <v>1.341621070215703</v>
+        <v>2.547669704768785</v>
       </c>
       <c r="F5" t="n">
-        <v>1.214905401540097</v>
+        <v>2.535321483732147</v>
       </c>
     </row>
     <row r="6">
@@ -568,19 +568,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.6924936979743261</v>
+        <v>1.509805436284917</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6298966221302366</v>
+        <v>1.542184752907285</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6069636238741689</v>
+        <v>1.552688270253863</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6115588787180845</v>
+        <v>1.555304830765864</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6117320399472587</v>
+        <v>1.588187828365613</v>
       </c>
     </row>
     <row r="8">
@@ -630,23 +630,23 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Nível Automação (Imobilizado/Receita)</t>
+          <t>Composição Endividamento (%)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.5855314210479801</v>
+        <v>72.30438869921596</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4515410100267366</v>
+        <v>72.67602517675823</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3972140824659633</v>
+        <v>72.15183776130478</v>
       </c>
       <c r="E10" t="n">
-        <v>0.343340788251323</v>
+        <v>71.81248303200837</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3576519808196515</v>
+        <v>71.71402927282512</v>
       </c>
     </row>
     <row r="11">
@@ -678,19 +678,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>68.07952325902824</v>
+        <v>49.22448312178091</v>
       </c>
       <c r="C12" t="n">
-        <v>61.6692255271138</v>
+        <v>44.81874187039704</v>
       </c>
       <c r="D12" t="n">
-        <v>56.03440238037519</v>
+        <v>40.42985109600502</v>
       </c>
       <c r="E12" t="n">
-        <v>52.6607145229394</v>
+        <v>37.81696668132022</v>
       </c>
       <c r="F12" t="n">
-        <v>47.91918537098822</v>
+        <v>34.36477862424982</v>
       </c>
     </row>
     <row r="13">
@@ -718,23 +718,209 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Alavancagem Financeira (PNC/PL)</t>
+          <t>Margem Operacional (%)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.777338748265412</v>
+        <v>-8.558666115731766</v>
       </c>
       <c r="C14" t="n">
-        <v>1.640271672050957</v>
+        <v>4.652544000903408</v>
       </c>
       <c r="D14" t="n">
-        <v>1.451796019768496</v>
+        <v>-2.369369379742759</v>
       </c>
       <c r="E14" t="n">
-        <v>1.341621070215703</v>
+        <v>5.831401193626308</v>
       </c>
       <c r="F14" t="n">
-        <v>1.214905401540097</v>
+        <v>10.64843742016398</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Margem Líquida (%)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-18.30911419157669</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-1.180509406717026</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-4.465961137152987</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.003981116115012</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5.430842226554105</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ROA (%)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-2.803384448797868</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.773398941590173</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-1.008247929558513</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2.927808167028303</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5.151783021070909</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>ROE (%)</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-21.65374177608858</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-1.646802552087117</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-6.824219169318738</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5.350693497321513</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9.288974679429796</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>GAO (Alavancagem Operacional)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>-16.67343635890709</v>
+      </c>
+      <c r="D18" t="n">
+        <v>103.0702857715295</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-33.23052961155219</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4.65579857716681</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>GAF (Alavancagem Financeira)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>0.5824369222021166</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-1.81640609962399</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4677093428249402</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9827286115496234</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>GAT (Alavancagem Total)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>-9.711224955414711</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-187.217495765394</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-15.54222916634379</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.575386471393852</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Var. % Receita</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>9.569885048300474</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-1.457105385130242</v>
+      </c>
+      <c r="E21" t="n">
+        <v>11.24872542319428</v>
+      </c>
+      <c r="F21" t="n">
+        <v>29.19169630181118</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Var. % EBIT</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>-159.5628693148944</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-150.1842684446086</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-373.8011032676776</v>
+      </c>
+      <c r="F22" t="n">
+        <v>135.9106581070581</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Var. % Lucro Líquido</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>-92.93530650150568</v>
+      </c>
+      <c r="D23" t="n">
+        <v>272.7956212703539</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-174.8302683565631</v>
+      </c>
+      <c r="F23" t="n">
+        <v>133.5632923363448</v>
       </c>
     </row>
   </sheetData>
@@ -748,7 +934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -886,221 +1072,199 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>PassivoCirculante</t>
+          <t>PassivoTotal</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16084627.91634959</v>
+        <v>69691047.31552862</v>
       </c>
       <c r="C7" t="n">
-        <v>18279637.44694333</v>
+        <v>65618880.5129077</v>
       </c>
       <c r="D7" t="n">
-        <v>18373669.44346336</v>
+        <v>57920929.21961301</v>
       </c>
       <c r="E7" t="n">
-        <v>18565945.7574</v>
+        <v>54612924.7336</v>
       </c>
       <c r="F7" t="n">
-        <v>27347016</v>
+        <v>73219718</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>PassivoNaoCirculante</t>
+          <t>PassivoCirculante</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>34305057.82322473</v>
+        <v>16084627.91634959</v>
       </c>
       <c r="C8" t="n">
-        <v>29409556.67532437</v>
+        <v>18279637.44694333</v>
       </c>
       <c r="D8" t="n">
-        <v>23417345.436912</v>
+        <v>18373669.44346336</v>
       </c>
       <c r="E8" t="n">
-        <v>20652951.5502</v>
+        <v>18565945.7574</v>
       </c>
       <c r="F8" t="n">
-        <v>25161794</v>
+        <v>27347016</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>PatrimonioLiquido</t>
+          <t>PassivoNaoCirculante</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>19301361.5759543</v>
+        <v>34305057.82322473</v>
       </c>
       <c r="C9" t="n">
-        <v>17929686.39064</v>
+        <v>29409556.67532437</v>
       </c>
       <c r="D9" t="n">
-        <v>16129914.33923764</v>
+        <v>23417345.436912</v>
       </c>
       <c r="E9" t="n">
-        <v>15394027.426</v>
+        <v>20652951.5502</v>
       </c>
       <c r="F9" t="n">
-        <v>20710908</v>
+        <v>25161794</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>ReceitaLiquida</t>
+          <t>PatrimonioLiquido</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>22827248.50145473</v>
+        <v>19301361.5759543</v>
       </c>
       <c r="C10" t="n">
-        <v>25011789.94273384</v>
+        <v>17929686.39064</v>
       </c>
       <c r="D10" t="n">
-        <v>24647341.8045608</v>
+        <v>16129914.33923764</v>
       </c>
       <c r="E10" t="n">
-        <v>27419853.60827202</v>
+        <v>15394027.426</v>
       </c>
       <c r="F10" t="n">
-        <v>35424174</v>
+        <v>20710908</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>LucroBruto</t>
+          <t>ReceitaLiquida</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2797304.76988113</v>
+        <v>22827248.50145473</v>
       </c>
       <c r="C11" t="n">
-        <v>3904740.967449251</v>
+        <v>25011789.94273384</v>
       </c>
       <c r="D11" t="n">
-        <v>4950725.889129187</v>
+        <v>24647341.8045608</v>
       </c>
       <c r="E11" t="n">
-        <v>4729220.957990627</v>
+        <v>27419853.60827202</v>
       </c>
       <c r="F11" t="n">
-        <v>6382234</v>
+        <v>35424174</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>LucroOperacional</t>
+          <t>LucroBruto</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-1953707.982647893</v>
+        <v>2797304.76988113</v>
       </c>
       <c r="C12" t="n">
-        <v>1163684.532499225</v>
+        <v>3904740.967449251</v>
       </c>
       <c r="D12" t="n">
-        <v>-583986.5696378001</v>
+        <v>4950725.889129187</v>
       </c>
       <c r="E12" t="n">
-        <v>1598961.670603361</v>
+        <v>4729220.957990627</v>
       </c>
       <c r="F12" t="n">
-        <v>3772121</v>
+        <v>6382234</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>LucroLiquido</t>
+          <t>LucroOperacional</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-4179466.994926325</v>
+        <v>-1953707.982647893</v>
       </c>
       <c r="C13" t="n">
-        <v>-295266.5330622761</v>
+        <v>1163684.532499225</v>
       </c>
       <c r="D13" t="n">
-        <v>-1100740.706332947</v>
+        <v>-583986.5696378001</v>
       </c>
       <c r="E13" t="n">
-        <v>823687.2244588722</v>
+        <v>1598961.670603361</v>
       </c>
       <c r="F13" t="n">
-        <v>1923831</v>
+        <v>3772121</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>PassivoTotal</t>
+          <t>LucroLiquido</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50389685.73957432</v>
+        <v>-4179466.994926325</v>
       </c>
       <c r="C14" t="n">
-        <v>47689194.1222677</v>
+        <v>-295266.5330622761</v>
       </c>
       <c r="D14" t="n">
-        <v>41791014.88037536</v>
+        <v>-1100740.706332947</v>
       </c>
       <c r="E14" t="n">
-        <v>39218897.3076</v>
+        <v>823687.2244588722</v>
       </c>
       <c r="F14" t="n">
-        <v>52508810</v>
+        <v>1923831</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>CapitalPermanente</t>
+          <t>AtivoPermanente</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>53606419.39917903</v>
+        <v>29141300.63507662</v>
       </c>
       <c r="C15" t="n">
-        <v>47339243.06596437</v>
+        <v>27650888.97605425</v>
       </c>
       <c r="D15" t="n">
-        <v>39547259.77614964</v>
+        <v>25044728.79473388</v>
       </c>
       <c r="E15" t="n">
-        <v>36046978.9762</v>
+        <v>23942405.2206</v>
       </c>
       <c r="F15" t="n">
-        <v>45872702</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>AtivoPermanente</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>13366071.25367216</v>
-      </c>
-      <c r="C16" t="n">
-        <v>11293848.89331861</v>
-      </c>
-      <c r="D16" t="n">
-        <v>9790271.260123599</v>
-      </c>
-      <c r="E16" t="n">
-        <v>9414354.1516</v>
-      </c>
-      <c r="F16" t="n">
-        <v>12669526</v>
+        <v>32892812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do índice de Imobilização do PL
</commit_message>
<xml_diff>
--- a/planilhas/Indicadores_Financeiros_Embraer.xlsx
+++ b/planilhas/Indicadores_Financeiros_Embraer.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,19 +568,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.509805436284917</v>
+        <v>1.406442047213015</v>
       </c>
       <c r="C7" t="n">
-        <v>1.542184752907285</v>
+        <v>1.429181031520963</v>
       </c>
       <c r="D7" t="n">
-        <v>1.552688270253863</v>
+        <v>1.406706186378151</v>
       </c>
       <c r="E7" t="n">
-        <v>1.555304830765864</v>
+        <v>1.38777482749692</v>
       </c>
       <c r="F7" t="n">
-        <v>1.588187828365613</v>
+        <v>1.373129995073128</v>
       </c>
     </row>
     <row r="8">
@@ -801,126 +801,6 @@
       </c>
       <c r="F17" t="n">
         <v>9.288974679429796</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>GAO (Alavancagem Operacional)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="n">
-        <v>-16.67343635890709</v>
-      </c>
-      <c r="D18" t="n">
-        <v>103.0702857715295</v>
-      </c>
-      <c r="E18" t="n">
-        <v>-33.23052961155219</v>
-      </c>
-      <c r="F18" t="n">
-        <v>4.65579857716681</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>GAF (Alavancagem Financeira)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="n">
-        <v>0.5824369222021166</v>
-      </c>
-      <c r="D19" t="n">
-        <v>-1.81640609962399</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.4677093428249402</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.9827286115496234</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>GAT (Alavancagem Total)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="n">
-        <v>-9.711224955414711</v>
-      </c>
-      <c r="D20" t="n">
-        <v>-187.217495765394</v>
-      </c>
-      <c r="E20" t="n">
-        <v>-15.54222916634379</v>
-      </c>
-      <c r="F20" t="n">
-        <v>4.575386471393852</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Var. % Receita</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>9.569885048300474</v>
-      </c>
-      <c r="D21" t="n">
-        <v>-1.457105385130242</v>
-      </c>
-      <c r="E21" t="n">
-        <v>11.24872542319428</v>
-      </c>
-      <c r="F21" t="n">
-        <v>29.19169630181118</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Var. % EBIT</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="n">
-        <v>-159.5628693148944</v>
-      </c>
-      <c r="D22" t="n">
-        <v>-150.1842684446086</v>
-      </c>
-      <c r="E22" t="n">
-        <v>-373.8011032676776</v>
-      </c>
-      <c r="F22" t="n">
-        <v>135.9106581070581</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Var. % Lucro Líquido</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="n">
-        <v>-92.93530650150568</v>
-      </c>
-      <c r="D23" t="n">
-        <v>272.7956212703539</v>
-      </c>
-      <c r="E23" t="n">
-        <v>-174.8302683565631</v>
-      </c>
-      <c r="F23" t="n">
-        <v>133.5632923363448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>